<commit_message>
Actualizacion logica flujo de autorizacion
</commit_message>
<xml_diff>
--- a/insert User.xlsx
+++ b/insert User.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\proyectoAlzate\Proyecto-Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F8B53E-39F7-45E8-B436-514350EEFD54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA784213-E150-469E-873F-8BDE0375CF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8D5DA090-16E5-4955-8F19-846849AFC9FE}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="70">
   <si>
     <t>alejandro</t>
   </si>
@@ -130,21 +129,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -236,6 +220,30 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>nikolas roa</t>
+  </si>
+  <si>
+    <t>1ro</t>
+  </si>
+  <si>
+    <t>2do</t>
+  </si>
+  <si>
+    <t>3ro</t>
+  </si>
+  <si>
+    <t>4to</t>
+  </si>
+  <si>
+    <t>5to</t>
+  </si>
+  <si>
+    <t>6to</t>
+  </si>
+  <si>
+    <t>7mo</t>
   </si>
 </sst>
 </file>
@@ -271,8 +279,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -298,8 +307,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{279760F1-8880-4A24-A6CE-7756D911D0A4}" name="Table1" displayName="Table1" ref="B4:G29" totalsRowShown="0">
-  <autoFilter ref="B4:G29" xr:uid="{171D490C-4B3F-4133-95FC-F34871F4C07F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{279760F1-8880-4A24-A6CE-7756D911D0A4}" name="Table1" displayName="Table1" ref="B4:G154" totalsRowShown="0">
+  <autoFilter ref="B4:G154" xr:uid="{171D490C-4B3F-4133-95FC-F34871F4C07F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{79861DF3-4C2F-4B40-B790-BA2C00460EEC}" name="id"/>
     <tableColumn id="2" xr3:uid="{AF0E8FD2-C5ED-45AE-AF33-C889E36688E0}" name="Nombre" dataDxfId="1"/>
@@ -307,7 +316,7 @@
     <tableColumn id="4" xr3:uid="{8E8AB922-0832-4457-80CD-C1FEA09B9A38}" name="Tipo"/>
     <tableColumn id="5" xr3:uid="{9EB2AF3E-6BA6-41D9-B994-2FBB319D8E04}" name="Permitido"/>
     <tableColumn id="6" xr3:uid="{831C1279-EB82-4AA6-A142-0BA6E0B32180}" name="Column1" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -669,17 +678,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DEF58A-1339-46C1-A358-C211AC41FDD0}">
-  <dimension ref="B4:G29"/>
+  <dimension ref="B4:G154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="114.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -699,7 +708,7 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -707,10 +716,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -719,8 +728,8 @@
         <v>0</v>
       </c>
       <c r="G5" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'andres roa NULL', 'A', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'nikolas roa', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -731,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -740,8 +749,8 @@
         <v>0</v>
       </c>
       <c r="G6" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'andres roa2 NULL', 'A', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa2 NULL', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -752,7 +761,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -761,8 +770,8 @@
         <v>0</v>
       </c>
       <c r="G7" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'andres roa NULL', 'A', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -773,7 +782,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -782,8 +791,8 @@
         <v>0</v>
       </c>
       <c r="G8" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'andres roa NULL', 'B', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '6to', 'N', 0,'');</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -794,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
         <v>30</v>
@@ -803,8 +812,8 @@
         <v>0</v>
       </c>
       <c r="G9" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'andres roa NULL', 'B', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -815,7 +824,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -824,8 +833,8 @@
         <v>0</v>
       </c>
       <c r="G10" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'andres roa NULL', 'B', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -836,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -845,8 +854,8 @@
         <v>0</v>
       </c>
       <c r="G11" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'camilo herrera', 'C', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'camilo herrera', '7mo', 'N', 0,'');</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -857,7 +866,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
@@ -866,8 +875,8 @@
         <v>0</v>
       </c>
       <c r="G12" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Rubiel Alberto Agudelo Echeverry', 'C', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Rubiel Alberto Agudelo Echeverry', '5to', 'N', 0,'');</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -878,7 +887,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -887,8 +896,8 @@
         <v>0</v>
       </c>
       <c r="G13" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Jhon Alexander Alvarez Puerta', 'C', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Alexander Alvarez Puerta', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -899,7 +908,7 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
@@ -908,8 +917,8 @@
         <v>0</v>
       </c>
       <c r="G14" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Alejandra Maria Arango Alvarez', 'D', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Alejandra Maria Arango Alvarez', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -920,7 +929,7 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
@@ -929,8 +938,8 @@
         <v>0</v>
       </c>
       <c r="G15" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Jaider Egidio Arango Arango', 'D', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jaider Egidio Arango Arango', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -941,7 +950,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -950,8 +959,8 @@
         <v>0</v>
       </c>
       <c r="G16" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Marlen Haygnes Arango Posada', 'D', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Marlen Haygnes Arango Posada', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -962,7 +971,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
@@ -971,8 +980,8 @@
         <v>0</v>
       </c>
       <c r="G17" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Johana Alexandra Atehortua Agudelo', 'E', 'N', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Johana Alexandra Atehortua Agudelo', '1ro', 'N', 0,'');</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -983,7 +992,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -992,8 +1001,8 @@
         <v>1</v>
       </c>
       <c r="G18" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Nai de Jesus Atehortua Atehortua', 'E', 'C', 1);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Nai de Jesus Atehortua Atehortua', '1ro', 'C', 1,'');</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -1004,7 +1013,7 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1013,8 +1022,8 @@
         <v>0</v>
       </c>
       <c r="G19" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Luz Elena Ayala Mira', 'E', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luz Elena Ayala Mira', '2do', 'C', 0,'');</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -1025,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -1034,8 +1043,8 @@
         <v>0</v>
       </c>
       <c r="G20" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Jhon Jairo Barrientos González', 'F', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Jairo Barrientos González', '2do', 'C', 0,'');</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -1046,7 +1055,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -1055,8 +1064,8 @@
         <v>0</v>
       </c>
       <c r="G21" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Mauro Albeiro Betancur Pineda', 'F', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Mauro Albeiro Betancur Pineda', '2do', 'C', 0,'');</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
@@ -1067,7 +1076,7 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -1076,8 +1085,8 @@
         <v>0</v>
       </c>
       <c r="G22" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Luis Reinaldo Bustamante Taborda', 'F', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luis Reinaldo Bustamante Taborda', '2do', 'C', 0,'');</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -1088,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
@@ -1097,8 +1106,8 @@
         <v>0</v>
       </c>
       <c r="G23" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'Yulieth Cardenas Chaverra', 'H', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Yulieth Cardenas Chaverra', '3ro', 'C', 0,'');</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -1109,7 +1118,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
@@ -1118,8 +1127,8 @@
         <v>0</v>
       </c>
       <c r="G24" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'votantea Alberto Agudelo Echeverry', 'H', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantea Alberto Agudelo Echeverry', '2do', 'C', 0,'');</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -1130,7 +1139,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
@@ -1139,8 +1148,8 @@
         <v>0</v>
       </c>
       <c r="G25" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'votanteb Alexander Alvarez Puerta', 'H', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanteb Alexander Alvarez Puerta', '2do', 'C', 0,'');</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -1151,7 +1160,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
@@ -1160,8 +1169,8 @@
         <v>0</v>
       </c>
       <c r="G26" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'votantec Maria Arango Alvarez', 'I', 'C', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantec Maria Arango Alvarez', '4to', 'C', 0,'');</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -1172,7 +1181,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
         <v>28</v>
@@ -1181,8 +1190,8 @@
         <v>0</v>
       </c>
       <c r="G27" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'votanted Egidio Arango Arango', 'I', 'A', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanted Egidio Arango Arango', '2do', 'A', 0,'');</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
@@ -1193,7 +1202,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
         <v>28</v>
@@ -1202,8 +1211,8 @@
         <v>1</v>
       </c>
       <c r="G28" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'votantee Haygnes Arango Posada', 'I', 'A', 1);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantee Haygnes Arango Posada', '2do', 'A', 1,'');</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -1214,7 +1223,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E29" t="s">
         <v>28</v>
@@ -1223,8 +1232,2633 @@
         <v>0</v>
       </c>
       <c r="G29" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],");")</f>
-        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`) VALUES (NULL, 'votantef Alexandra Atehortua Agudelo', 'I', 'A', 0);</v>
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantef Alexandra Atehortua Agudelo', 'I', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'nikolas roa', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa2 NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>28</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '6to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>31</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'camilo herrera', '7mo', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>33</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Rubiel Alberto Agudelo Echeverry', '5to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>34</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Alexander Alvarez Puerta', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>35</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Alejandra Maria Arango Alvarez', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>36</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jaider Egidio Arango Arango', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>37</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Marlen Haygnes Arango Posada', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>38</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Johana Alexandra Atehortua Agudelo', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>39</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Nai de Jesus Atehortua Atehortua', '1ro', 'C', 1,'');</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>40</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luz Elena Ayala Mira', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>41</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Jairo Barrientos González', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>42</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Mauro Albeiro Betancur Pineda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>43</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luis Reinaldo Bustamante Taborda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>44</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Yulieth Cardenas Chaverra', '3ro', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>45</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantea Alberto Agudelo Echeverry', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>46</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanteb Alexander Alvarez Puerta', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>47</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantec Maria Arango Alvarez', '4to', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>48</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanted Egidio Arango Arango', '2do', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>49</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantee Haygnes Arango Posada', '2do', 'A', 1,'');</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>50</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantef Alexandra Atehortua Agudelo', 'I', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>51</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'nikolas roa', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>52</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa2 NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>53</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>54</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '6to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>55</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>56</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>57</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'camilo herrera', '7mo', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>58</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Rubiel Alberto Agudelo Echeverry', '5to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>59</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Alexander Alvarez Puerta', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>60</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>63</v>
+      </c>
+      <c r="E64" t="s">
+        <v>30</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Alejandra Maria Arango Alvarez', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>61</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" t="s">
+        <v>30</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jaider Egidio Arango Arango', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>62</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Marlen Haygnes Arango Posada', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>63</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Johana Alexandra Atehortua Agudelo', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>64</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Nai de Jesus Atehortua Atehortua', '1ro', 'C', 1,'');</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>65</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" t="s">
+        <v>29</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luz Elena Ayala Mira', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>66</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" t="s">
+        <v>29</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Jairo Barrientos González', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>67</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Mauro Albeiro Betancur Pineda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>68</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" t="s">
+        <v>64</v>
+      </c>
+      <c r="E72" t="s">
+        <v>29</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luis Reinaldo Bustamante Taborda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>69</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" t="s">
+        <v>65</v>
+      </c>
+      <c r="E73" t="s">
+        <v>29</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Yulieth Cardenas Chaverra', '3ro', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>70</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" t="s">
+        <v>29</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantea Alberto Agudelo Echeverry', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>71</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" t="s">
+        <v>29</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanteb Alexander Alvarez Puerta', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>72</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" t="s">
+        <v>66</v>
+      </c>
+      <c r="E76" t="s">
+        <v>29</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantec Maria Arango Alvarez', '4to', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>73</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanted Egidio Arango Arango', '2do', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>74</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>64</v>
+      </c>
+      <c r="E78" t="s">
+        <v>28</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantee Haygnes Arango Posada', '2do', 'A', 1,'');</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>75</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D79" t="s">
+        <v>31</v>
+      </c>
+      <c r="E79" t="s">
+        <v>28</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantef Alexandra Atehortua Agudelo', 'I', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>76</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80" t="s">
+        <v>63</v>
+      </c>
+      <c r="E80" t="s">
+        <v>30</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'nikolas roa', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>77</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>63</v>
+      </c>
+      <c r="E81" t="s">
+        <v>30</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa2 NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>78</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>63</v>
+      </c>
+      <c r="E82" t="s">
+        <v>30</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>79</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>68</v>
+      </c>
+      <c r="E83" t="s">
+        <v>30</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '6to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>80</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>63</v>
+      </c>
+      <c r="E84" t="s">
+        <v>30</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>81</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" t="s">
+        <v>30</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>82</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>69</v>
+      </c>
+      <c r="E86" t="s">
+        <v>30</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'camilo herrera', '7mo', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>83</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" t="s">
+        <v>67</v>
+      </c>
+      <c r="E87" t="s">
+        <v>30</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Rubiel Alberto Agudelo Echeverry', '5to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>84</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" t="s">
+        <v>63</v>
+      </c>
+      <c r="E88" t="s">
+        <v>30</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Alexander Alvarez Puerta', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>85</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" t="s">
+        <v>63</v>
+      </c>
+      <c r="E89" t="s">
+        <v>30</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Alejandra Maria Arango Alvarez', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>86</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" t="s">
+        <v>63</v>
+      </c>
+      <c r="E90" t="s">
+        <v>30</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jaider Egidio Arango Arango', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>87</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Marlen Haygnes Arango Posada', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>88</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" t="s">
+        <v>63</v>
+      </c>
+      <c r="E92" t="s">
+        <v>30</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Johana Alexandra Atehortua Agudelo', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>89</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" t="s">
+        <v>63</v>
+      </c>
+      <c r="E93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Nai de Jesus Atehortua Atehortua', '1ro', 'C', 1,'');</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>90</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" t="s">
+        <v>64</v>
+      </c>
+      <c r="E94" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luz Elena Ayala Mira', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>91</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95" t="s">
+        <v>64</v>
+      </c>
+      <c r="E95" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Jairo Barrientos González', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>92</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" t="s">
+        <v>64</v>
+      </c>
+      <c r="E96" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Mauro Albeiro Betancur Pineda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>93</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E97" t="s">
+        <v>29</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luis Reinaldo Bustamante Taborda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>94</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" t="s">
+        <v>65</v>
+      </c>
+      <c r="E98" t="s">
+        <v>29</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Yulieth Cardenas Chaverra', '3ro', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>95</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D99" t="s">
+        <v>64</v>
+      </c>
+      <c r="E99" t="s">
+        <v>29</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantea Alberto Agudelo Echeverry', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>96</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D100" t="s">
+        <v>64</v>
+      </c>
+      <c r="E100" t="s">
+        <v>29</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanteb Alexander Alvarez Puerta', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>97</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" t="s">
+        <v>66</v>
+      </c>
+      <c r="E101" t="s">
+        <v>29</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantec Maria Arango Alvarez', '4to', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>98</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D102" t="s">
+        <v>64</v>
+      </c>
+      <c r="E102" t="s">
+        <v>28</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanted Egidio Arango Arango', '2do', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>99</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D103" t="s">
+        <v>64</v>
+      </c>
+      <c r="E103" t="s">
+        <v>28</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantee Haygnes Arango Posada', '2do', 'A', 1,'');</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>100</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D104" t="s">
+        <v>31</v>
+      </c>
+      <c r="E104" t="s">
+        <v>28</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantef Alexandra Atehortua Agudelo', 'I', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>101</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D105" t="s">
+        <v>63</v>
+      </c>
+      <c r="E105" t="s">
+        <v>30</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'nikolas roa', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>102</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" t="s">
+        <v>63</v>
+      </c>
+      <c r="E106" t="s">
+        <v>30</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa2 NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>103</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" t="s">
+        <v>63</v>
+      </c>
+      <c r="E107" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>104</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
+        <v>68</v>
+      </c>
+      <c r="E108" t="s">
+        <v>30</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '6to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>105</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" t="s">
+        <v>63</v>
+      </c>
+      <c r="E109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>106</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" t="s">
+        <v>63</v>
+      </c>
+      <c r="E110" t="s">
+        <v>30</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>107</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" t="s">
+        <v>69</v>
+      </c>
+      <c r="E111" t="s">
+        <v>30</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'camilo herrera', '7mo', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>108</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D112" t="s">
+        <v>67</v>
+      </c>
+      <c r="E112" t="s">
+        <v>30</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Rubiel Alberto Agudelo Echeverry', '5to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>109</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" t="s">
+        <v>63</v>
+      </c>
+      <c r="E113" t="s">
+        <v>30</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Alexander Alvarez Puerta', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>110</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" t="s">
+        <v>63</v>
+      </c>
+      <c r="E114" t="s">
+        <v>30</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Alejandra Maria Arango Alvarez', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>111</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D115" t="s">
+        <v>63</v>
+      </c>
+      <c r="E115" t="s">
+        <v>30</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jaider Egidio Arango Arango', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>112</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" t="s">
+        <v>63</v>
+      </c>
+      <c r="E116" t="s">
+        <v>30</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Marlen Haygnes Arango Posada', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>113</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" t="s">
+        <v>63</v>
+      </c>
+      <c r="E117" t="s">
+        <v>30</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Johana Alexandra Atehortua Agudelo', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>114</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D118" t="s">
+        <v>63</v>
+      </c>
+      <c r="E118" t="s">
+        <v>29</v>
+      </c>
+      <c r="F118">
+        <v>1</v>
+      </c>
+      <c r="G118" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Nai de Jesus Atehortua Atehortua', '1ro', 'C', 1,'');</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>115</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D119" t="s">
+        <v>64</v>
+      </c>
+      <c r="E119" t="s">
+        <v>29</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luz Elena Ayala Mira', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>116</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D120" t="s">
+        <v>64</v>
+      </c>
+      <c r="E120" t="s">
+        <v>29</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="G120" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Jairo Barrientos González', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>117</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D121" t="s">
+        <v>64</v>
+      </c>
+      <c r="E121" t="s">
+        <v>29</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Mauro Albeiro Betancur Pineda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>118</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D122" t="s">
+        <v>64</v>
+      </c>
+      <c r="E122" t="s">
+        <v>29</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luis Reinaldo Bustamante Taborda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>119</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D123" t="s">
+        <v>65</v>
+      </c>
+      <c r="E123" t="s">
+        <v>29</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Yulieth Cardenas Chaverra', '3ro', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>120</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D124" t="s">
+        <v>64</v>
+      </c>
+      <c r="E124" t="s">
+        <v>29</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="G124" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantea Alberto Agudelo Echeverry', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>121</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" t="s">
+        <v>64</v>
+      </c>
+      <c r="E125" t="s">
+        <v>29</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanteb Alexander Alvarez Puerta', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>122</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D126" t="s">
+        <v>66</v>
+      </c>
+      <c r="E126" t="s">
+        <v>29</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+      <c r="G126" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantec Maria Arango Alvarez', '4to', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>123</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" t="s">
+        <v>64</v>
+      </c>
+      <c r="E127" t="s">
+        <v>28</v>
+      </c>
+      <c r="F127">
+        <v>0</v>
+      </c>
+      <c r="G127" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanted Egidio Arango Arango', '2do', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>124</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D128" t="s">
+        <v>64</v>
+      </c>
+      <c r="E128" t="s">
+        <v>28</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="G128" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantee Haygnes Arango Posada', '2do', 'A', 1,'');</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>125</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D129" t="s">
+        <v>31</v>
+      </c>
+      <c r="E129" t="s">
+        <v>28</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+      <c r="G129" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantef Alexandra Atehortua Agudelo', 'I', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>126</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D130" t="s">
+        <v>63</v>
+      </c>
+      <c r="E130" t="s">
+        <v>30</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'nikolas roa', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>127</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" t="s">
+        <v>63</v>
+      </c>
+      <c r="E131" t="s">
+        <v>30</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+      <c r="G131" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa2 NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>128</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132" t="s">
+        <v>63</v>
+      </c>
+      <c r="E132" t="s">
+        <v>30</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>129</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133" t="s">
+        <v>68</v>
+      </c>
+      <c r="E133" t="s">
+        <v>30</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="G133" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '6to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>130</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134" t="s">
+        <v>63</v>
+      </c>
+      <c r="E134" t="s">
+        <v>30</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+      <c r="G134" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>131</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" t="s">
+        <v>63</v>
+      </c>
+      <c r="E135" t="s">
+        <v>30</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="G135" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'andres roa NULL', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>132</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" t="s">
+        <v>69</v>
+      </c>
+      <c r="E136" t="s">
+        <v>30</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'camilo herrera', '7mo', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>133</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D137" t="s">
+        <v>67</v>
+      </c>
+      <c r="E137" t="s">
+        <v>30</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Rubiel Alberto Agudelo Echeverry', '5to', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>134</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D138" t="s">
+        <v>63</v>
+      </c>
+      <c r="E138" t="s">
+        <v>30</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="G138" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Alexander Alvarez Puerta', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>135</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D139" t="s">
+        <v>63</v>
+      </c>
+      <c r="E139" t="s">
+        <v>30</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Alejandra Maria Arango Alvarez', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>136</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" t="s">
+        <v>63</v>
+      </c>
+      <c r="E140" t="s">
+        <v>30</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jaider Egidio Arango Arango', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>137</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" t="s">
+        <v>63</v>
+      </c>
+      <c r="E141" t="s">
+        <v>30</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Marlen Haygnes Arango Posada', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>138</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142" t="s">
+        <v>63</v>
+      </c>
+      <c r="E142" t="s">
+        <v>30</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Johana Alexandra Atehortua Agudelo', '1ro', 'N', 0,'');</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>139</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D143" t="s">
+        <v>63</v>
+      </c>
+      <c r="E143" t="s">
+        <v>29</v>
+      </c>
+      <c r="F143">
+        <v>1</v>
+      </c>
+      <c r="G143" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Nai de Jesus Atehortua Atehortua', '1ro', 'C', 1,'');</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>140</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D144" t="s">
+        <v>64</v>
+      </c>
+      <c r="E144" t="s">
+        <v>29</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luz Elena Ayala Mira', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>141</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D145" t="s">
+        <v>64</v>
+      </c>
+      <c r="E145" t="s">
+        <v>29</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Jhon Jairo Barrientos González', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>142</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D146" t="s">
+        <v>64</v>
+      </c>
+      <c r="E146" t="s">
+        <v>29</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Mauro Albeiro Betancur Pineda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>143</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D147" t="s">
+        <v>64</v>
+      </c>
+      <c r="E147" t="s">
+        <v>29</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+      <c r="G147" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Luis Reinaldo Bustamante Taborda', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>144</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D148" t="s">
+        <v>65</v>
+      </c>
+      <c r="E148" t="s">
+        <v>29</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="G148" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'Yulieth Cardenas Chaverra', '3ro', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>145</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D149" t="s">
+        <v>64</v>
+      </c>
+      <c r="E149" t="s">
+        <v>29</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantea Alberto Agudelo Echeverry', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B150">
+        <v>146</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D150" t="s">
+        <v>64</v>
+      </c>
+      <c r="E150" t="s">
+        <v>29</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanteb Alexander Alvarez Puerta', '2do', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B151">
+        <v>147</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D151" t="s">
+        <v>66</v>
+      </c>
+      <c r="E151" t="s">
+        <v>29</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantec Maria Arango Alvarez', '4to', 'C', 0,'');</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B152">
+        <v>148</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D152" t="s">
+        <v>64</v>
+      </c>
+      <c r="E152" t="s">
+        <v>28</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votanted Egidio Arango Arango', '2do', 'A', 0,'');</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B153">
+        <v>149</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153" t="s">
+        <v>64</v>
+      </c>
+      <c r="E153" t="s">
+        <v>28</v>
+      </c>
+      <c r="F153">
+        <v>1</v>
+      </c>
+      <c r="G153" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantee Haygnes Arango Posada', '2do', 'A', 1,'');</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B154">
+        <v>150</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D154" t="s">
+        <v>31</v>
+      </c>
+      <c r="E154" t="s">
+        <v>28</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, '",Table1[[#This Row],[Nombre]],"', '",Table1[[#This Row],[Grupo]],"', '",Table1[[#This Row],[Tipo]],"', ",Table1[[#This Row],[Permitido]],",'');")</f>
+        <v>INSERT INTO `estudiantes` (`id`, `Nombre`, `Grupo`, `Tipo`, `Autorizado`,`Descripcion`) VALUES (NULL, 'votantef Alexandra Atehortua Agudelo', 'I', 'A', 0,'');</v>
       </c>
     </row>
   </sheetData>
@@ -1256,122 +3890,122 @@
     </row>
     <row r="5" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1399,13 +4033,13 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="5:8" x14ac:dyDescent="0.3">
@@ -1416,7 +4050,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="5:8" x14ac:dyDescent="0.3">
@@ -1427,7 +4061,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.3">
@@ -1438,7 +4072,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>